<commit_message>
Du kan ta upp och använda lost souls!
Q för sacrifice, E för free
</commit_message>
<xml_diff>
--- a/Code/CollisionTable.xlsx
+++ b/Code/CollisionTable.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="11">
   <si>
     <t>player</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>firefoebullet</t>
+  </si>
+  <si>
+    <t>lostsoul</t>
   </si>
 </sst>
 </file>
@@ -384,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -397,10 +400,10 @@
     <col min="7" max="7" width="18.21875" customWidth="1"/>
     <col min="8" max="8" width="17.88671875" customWidth="1"/>
     <col min="9" max="9" width="16.21875" customWidth="1"/>
-    <col min="10" max="10" width="22.21875" customWidth="1"/>
+    <col min="10" max="10" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -425,8 +428,11 @@
       <c r="I1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -454,8 +460,11 @@
       <c r="I2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -483,8 +492,11 @@
       <c r="I3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -512,8 +524,11 @@
       <c r="I4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -541,8 +556,11 @@
       <c r="I5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -570,8 +588,11 @@
       <c r="I6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -599,8 +620,11 @@
       <c r="I7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -628,8 +652,11 @@
       <c r="I8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -655,6 +682,41 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Altare i Alpha Jian(ej utsatta på banan dock) etc
När altarnas sprites är klara sätter vi ut dem på banan och fixar deras
collision boxes.
Lite skit i Nicolina mappen uppdateras också.
</commit_message>
<xml_diff>
--- a/Code/CollisionTable.xlsx
+++ b/Code/CollisionTable.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="12">
   <si>
     <t>player</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>lostsoul</t>
+  </si>
+  <si>
+    <t>altar</t>
   </si>
 </sst>
 </file>
@@ -387,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -403,7 +406,7 @@
     <col min="10" max="10" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -431,8 +434,11 @@
       <c r="J1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -463,8 +469,11 @@
       <c r="J2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -495,8 +504,11 @@
       <c r="J3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -527,8 +539,11 @@
       <c r="J4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -559,8 +574,11 @@
       <c r="J5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -591,8 +609,11 @@
       <c r="J6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -623,8 +644,11 @@
       <c r="J7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -655,8 +679,11 @@
       <c r="J8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -687,8 +714,11 @@
       <c r="J9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -717,6 +747,44 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bug fixes + knockback + Start on walls
Bug fixes:
* fixat en bug när man sköt 2 skott samtidigt (i varandra)
* Ändrade om i hur collisionmap:en fungerar (nu behöver man bara skriva
in en form av collision. T.ex. Player->firefoe | och inte
player->firefoe, firefoe->player)
implementerade knockback till spelaren (mot fiender och väggar)
och har en grov start på väggar, påminn mig om att ha en frågestund
kring dem.
</commit_message>
<xml_diff>
--- a/Code/CollisionTable.xlsx
+++ b/Code/CollisionTable.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="13">
   <si>
     <t>player</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>altar</t>
+  </si>
+  <si>
+    <t>wall</t>
   </si>
 </sst>
 </file>
@@ -390,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -406,7 +409,7 @@
     <col min="10" max="10" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -437,8 +440,11 @@
       <c r="K1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -472,8 +478,11 @@
       <c r="K2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -507,8 +516,11 @@
       <c r="K3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -542,8 +554,11 @@
       <c r="K4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -577,8 +592,11 @@
       <c r="K5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -612,8 +630,11 @@
       <c r="K6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -647,8 +668,11 @@
       <c r="K7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -682,8 +706,11 @@
       <c r="K8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -717,8 +744,11 @@
       <c r="K9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -752,8 +782,11 @@
       <c r="K10" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -785,6 +818,47 @@
         <v>1</v>
       </c>
       <c r="K11" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" t="s">
+        <v>1</v>
+      </c>
+      <c r="L12" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>